<commit_message>
add optional parameters to the Excel import
</commit_message>
<xml_diff>
--- a/static/file/product_database_import_template.xlsx
+++ b/static/file/product_database_import_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -54,33 +54,80 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If set, a lifecycle state is shown in the product database. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>product id</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>vendor</t>
-  </si>
-  <si>
-    <t>list price</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>EoX update timestamp</t>
+  </si>
+  <si>
+    <t>EoL announcement date</t>
+  </si>
+  <si>
+    <t>End of Sale date</t>
+  </si>
+  <si>
+    <t>End of new service attachment date</t>
+  </si>
+  <si>
+    <t>End of SW maintenance date</t>
+  </si>
+  <si>
+    <t>End of Routing failure analysis date</t>
+  </si>
+  <si>
+    <t>End of Service contract renewal date</t>
+  </si>
+  <si>
+    <t>End of Security/Vulnerability support date</t>
+  </si>
+  <si>
+    <t>Last date of support</t>
+  </si>
+  <si>
+    <t>EoL note URL (friendly name)</t>
+  </si>
+  <si>
+    <t>EoL note URL</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Vendor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,6 +150,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,10 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,33 +517,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add product group to excel import
</commit_message>
<xml_diff>
--- a/static/file/product_database_import_template.xlsx
+++ b/static/file/product_database_import_template.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoelsner/Projects/coding-projects-on-github/product-database/src/source/static/file/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -54,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>EoX update timestamp</t>
   </si>
@@ -121,13 +129,16 @@
   </si>
   <si>
     <t>Vendor</t>
+  </si>
+  <si>
+    <t>Product Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -150,13 +161,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,24 +178,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -517,32 +536,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -558,37 +577,40 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -596,10 +618,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add internal product ID to data model
</commit_message>
<xml_diff>
--- a/static/file/product_database_import_template.xlsx
+++ b/static/file/product_database_import_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>EoX update timestamp</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Product Group</t>
+  </si>
+  <si>
+    <t>internal product ID</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -536,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,9 +562,10 @@
     <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -612,6 +616,9 @@
       </c>
       <c r="Q1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>